<commit_message>
Corrected code for g expl & the arguments for the code in the separate excel file
I corrected the code for g explanation according to TIm's feedback
</commit_message>
<xml_diff>
--- a/data/coding explanations_AI.xlsx
+++ b/data/coding explanations_AI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RES KP\Clients\Contracts\World Bank\ESG\October\Latest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R working directory\ESG_availability\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FFAAF7-8B27-4ABF-9836-34C7610F77B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA6882A-7003-4648-86FC-CE186F81AB55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B45AD726-65CD-4CBE-85A5-FE32CC3EFE12}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="329">
   <si>
     <t>cetsid</t>
   </si>
@@ -963,18 +963,9 @@
     <t>Indicator is updated using raw data from 2+ years prior MRV 2017 c; data si gepgraphicallly limited, 22 small countries missing g</t>
   </si>
   <si>
-    <t>Indicator is updated using raw data from 2+ years prior - MRV 2017 c; data is geographically limited, 19 small and 23 rich countries missing g</t>
-  </si>
-  <si>
     <t>Indicator is updated using raw data from 2+ years prior - MRV 2017, c; data is geographically limited 22 small countries missing g</t>
   </si>
   <si>
-    <t>Data is geograhically limited, 19 small countries missing - g</t>
-  </si>
-  <si>
-    <t>Data is geograhically limited - g</t>
-  </si>
-  <si>
     <t>Indicator is updated using raw data from 2+ years prior - MRV 2017, c; rich countries missing - 71 g</t>
   </si>
   <si>
@@ -990,21 +981,9 @@
     <t>MRV 2015 - c</t>
   </si>
   <si>
-    <t>MRV 2017 - c; 72 countries gaps; 18 small - g</t>
-  </si>
-  <si>
-    <t>17 small countries - g</t>
-  </si>
-  <si>
-    <t>23 small countries missing - g</t>
-  </si>
-  <si>
     <t>24 small countries missing - g</t>
   </si>
   <si>
-    <t>14 small countries missing - g</t>
-  </si>
-  <si>
     <t>licensing lags e</t>
   </si>
   <si>
@@ -1017,9 +996,6 @@
     <t>licensing lags e; geographical limitations - 23 small countries missing g</t>
   </si>
   <si>
-    <t>licensing lags e; geographical limitations - 19 small countries missing</t>
-  </si>
-  <si>
     <t>indicator not being updated b; geographical limitations 21 countries missing g</t>
   </si>
   <si>
@@ -1036,6 +1012,15 @@
   </si>
   <si>
     <t>24 countries missing g; dependence on microdata f</t>
+  </si>
+  <si>
+    <t>licensing lags e; MRV - 2015</t>
+  </si>
+  <si>
+    <t>Indicator is updated using raw data from 2+ years prior - MRV 2017 c;</t>
+  </si>
+  <si>
+    <t>MRV 2018</t>
   </si>
 </sst>
 </file>
@@ -1390,7 +1375,9 @@
   <dimension ref="A1:M136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="M86" sqref="M86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1930,7 +1917,7 @@
         <v>281</v>
       </c>
       <c r="M13" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1971,7 +1958,7 @@
         <v>281</v>
       </c>
       <c r="M14" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -2012,7 +1999,7 @@
         <v>281</v>
       </c>
       <c r="M15" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -2053,7 +2040,7 @@
         <v>281</v>
       </c>
       <c r="M16" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -2094,7 +2081,7 @@
         <v>281</v>
       </c>
       <c r="M17" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -2114,7 +2101,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -2126,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -2135,7 +2122,7 @@
         <v>281</v>
       </c>
       <c r="M18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -2176,7 +2163,7 @@
         <v>281</v>
       </c>
       <c r="M19" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2258,7 +2245,7 @@
         <v>281</v>
       </c>
       <c r="M21" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -2299,7 +2286,7 @@
         <v>281</v>
       </c>
       <c r="M22" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2381,7 +2368,7 @@
         <v>281</v>
       </c>
       <c r="M24" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -2422,7 +2409,7 @@
         <v>281</v>
       </c>
       <c r="M25" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -2463,7 +2450,7 @@
         <v>281</v>
       </c>
       <c r="M26" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -2504,7 +2491,7 @@
         <v>281</v>
       </c>
       <c r="M27" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -2668,7 +2655,7 @@
         <v>281</v>
       </c>
       <c r="M31" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -2832,7 +2819,7 @@
         <v>281</v>
       </c>
       <c r="M35" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -2873,7 +2860,7 @@
         <v>281</v>
       </c>
       <c r="M36" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -2914,7 +2901,7 @@
         <v>281</v>
       </c>
       <c r="M37" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -2996,7 +2983,7 @@
         <v>281</v>
       </c>
       <c r="M39" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
@@ -3356,7 +3343,7 @@
         <v>0</v>
       </c>
       <c r="J48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K48">
         <v>0</v>
@@ -3365,7 +3352,7 @@
         <v>283</v>
       </c>
       <c r="M48" t="s">
-        <v>309</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
@@ -3406,7 +3393,7 @@
         <v>283</v>
       </c>
       <c r="M49" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
@@ -3438,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="J50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K50">
         <v>0</v>
@@ -3447,7 +3434,7 @@
         <v>285</v>
       </c>
       <c r="M50" t="s">
-        <v>311</v>
+        <v>328</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
@@ -3561,7 +3548,7 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -3570,7 +3557,7 @@
         <v>285</v>
       </c>
       <c r="M53" t="s">
-        <v>311</v>
+        <v>328</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
@@ -3602,7 +3589,7 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K54">
         <v>0</v>
@@ -3611,7 +3598,7 @@
         <v>285</v>
       </c>
       <c r="M54" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
@@ -3643,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="J55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55">
         <v>0</v>
@@ -3652,7 +3639,7 @@
         <v>285</v>
       </c>
       <c r="M55" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
@@ -3684,7 +3671,7 @@
         <v>0</v>
       </c>
       <c r="J56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56">
         <v>0</v>
@@ -3693,7 +3680,7 @@
         <v>285</v>
       </c>
       <c r="M56" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
@@ -3725,7 +3712,7 @@
         <v>0</v>
       </c>
       <c r="J57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -3734,7 +3721,7 @@
         <v>285</v>
       </c>
       <c r="M57" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
@@ -3775,7 +3762,7 @@
         <v>285</v>
       </c>
       <c r="M58" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
@@ -3816,7 +3803,7 @@
         <v>285</v>
       </c>
       <c r="M59" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
@@ -3857,7 +3844,7 @@
         <v>285</v>
       </c>
       <c r="M60" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
@@ -3898,7 +3885,7 @@
         <v>285</v>
       </c>
       <c r="M61" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
@@ -3939,7 +3926,7 @@
         <v>285</v>
       </c>
       <c r="M62" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
@@ -3980,7 +3967,7 @@
         <v>285</v>
       </c>
       <c r="M63" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
@@ -4021,7 +4008,7 @@
         <v>285</v>
       </c>
       <c r="M64" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
@@ -4062,7 +4049,7 @@
         <v>285</v>
       </c>
       <c r="M65" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
@@ -4103,7 +4090,7 @@
         <v>286</v>
       </c>
       <c r="M66" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
@@ -4267,7 +4254,7 @@
         <v>286</v>
       </c>
       <c r="M70" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
@@ -4387,7 +4374,7 @@
         <v>287</v>
       </c>
       <c r="M73" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
@@ -4510,7 +4497,7 @@
         <v>287</v>
       </c>
       <c r="M76" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
@@ -4551,7 +4538,7 @@
         <v>287</v>
       </c>
       <c r="M77" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
@@ -4592,7 +4579,7 @@
         <v>287</v>
       </c>
       <c r="M78" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
@@ -4633,7 +4620,7 @@
         <v>287</v>
       </c>
       <c r="M79" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
@@ -4674,7 +4661,7 @@
         <v>287</v>
       </c>
       <c r="M80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
@@ -4715,7 +4702,7 @@
         <v>287</v>
       </c>
       <c r="M81" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
@@ -4756,7 +4743,7 @@
         <v>287</v>
       </c>
       <c r="M82" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
@@ -4797,7 +4784,7 @@
         <v>283</v>
       </c>
       <c r="M83" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
@@ -4817,7 +4804,7 @@
         <v>0</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -4829,7 +4816,7 @@
         <v>0</v>
       </c>
       <c r="J84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K84">
         <v>0</v>
@@ -4838,7 +4825,7 @@
         <v>287</v>
       </c>
       <c r="M84" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
@@ -4858,7 +4845,7 @@
         <v>0</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -4870,7 +4857,7 @@
         <v>0</v>
       </c>
       <c r="J85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K85">
         <v>0</v>
@@ -4879,7 +4866,7 @@
         <v>287</v>
       </c>
       <c r="M85" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.3">
@@ -4920,7 +4907,7 @@
         <v>283</v>
       </c>
       <c r="M86" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
@@ -5002,7 +4989,7 @@
         <v>283</v>
       </c>
       <c r="M88" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.3">
@@ -5043,7 +5030,7 @@
         <v>283</v>
       </c>
       <c r="M89" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.3">
@@ -5084,7 +5071,7 @@
         <v>284</v>
       </c>
       <c r="M90" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.3">
@@ -5494,7 +5481,7 @@
         <v>283</v>
       </c>
       <c r="M100" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.3">
@@ -5535,7 +5522,7 @@
         <v>283</v>
       </c>
       <c r="M101" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.3">
@@ -5649,7 +5636,7 @@
         <v>0</v>
       </c>
       <c r="J104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K104">
         <v>0</v>
@@ -5658,7 +5645,7 @@
         <v>285</v>
       </c>
       <c r="M104" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.3">
@@ -5740,7 +5727,7 @@
         <v>287</v>
       </c>
       <c r="M106" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.3">
@@ -5781,7 +5768,7 @@
         <v>287</v>
       </c>
       <c r="M107" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.3">
@@ -5822,7 +5809,7 @@
         <v>287</v>
       </c>
       <c r="M108" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
@@ -5904,7 +5891,7 @@
         <v>286</v>
       </c>
       <c r="M110" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.3">
@@ -5936,7 +5923,7 @@
         <v>0</v>
       </c>
       <c r="J111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K111">
         <v>0</v>
@@ -5945,7 +5932,7 @@
         <v>285</v>
       </c>
       <c r="M111" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
@@ -5986,7 +5973,7 @@
         <v>288</v>
       </c>
       <c r="M112" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.3">
@@ -6027,7 +6014,7 @@
         <v>288</v>
       </c>
       <c r="M113" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.3">
@@ -6068,7 +6055,7 @@
         <v>281</v>
       </c>
       <c r="M114" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.3">
@@ -6109,7 +6096,7 @@
         <v>287</v>
       </c>
       <c r="M115" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.3">
@@ -6141,7 +6128,7 @@
         <v>0</v>
       </c>
       <c r="J116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K116">
         <v>0</v>
@@ -6150,7 +6137,7 @@
         <v>285</v>
       </c>
       <c r="M116" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.3">
@@ -6191,7 +6178,7 @@
         <v>288</v>
       </c>
       <c r="M117" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.3">
@@ -6273,7 +6260,7 @@
         <v>284</v>
       </c>
       <c r="M119" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.3">
@@ -6601,7 +6588,7 @@
         <v>288</v>
       </c>
       <c r="M127" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.3">
@@ -6642,7 +6629,7 @@
         <v>285</v>
       </c>
       <c r="M128" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.3">
@@ -6674,7 +6661,7 @@
         <v>0</v>
       </c>
       <c r="J129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K129">
         <v>0</v>
@@ -6683,7 +6670,7 @@
         <v>285</v>
       </c>
       <c r="M129" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.3">
@@ -6724,7 +6711,7 @@
         <v>283</v>
       </c>
       <c r="M130" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.3">
@@ -6806,7 +6793,7 @@
         <v>285</v>
       </c>
       <c r="M132" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.3">
@@ -6847,7 +6834,7 @@
         <v>285</v>
       </c>
       <c r="M133" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.3">
@@ -6888,7 +6875,7 @@
         <v>283</v>
       </c>
       <c r="M134" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.3">
@@ -6929,7 +6916,7 @@
         <v>281</v>
       </c>
       <c r="M135" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.3">
@@ -6970,7 +6957,7 @@
         <v>288</v>
       </c>
       <c r="M136" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated coding for retirement age variable
Moved to 0 all code as it has data for 2018, a database and was updated in 2019
</commit_message>
<xml_diff>
--- a/data/coding explanations_AI.xlsx
+++ b/data/coding explanations_AI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R working directory\ESG_availability\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA6882A-7003-4648-86FC-CE186F81AB55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA65468-88B3-427A-8DF9-90536EBDC5B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B45AD726-65CD-4CBE-85A5-FE32CC3EFE12}"/>
   </bookViews>
@@ -1374,10 +1374,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C5F7576-3365-4997-A4EE-300F068BDE5E}">
   <dimension ref="A1:M136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="M86" sqref="M86"/>
+      <selection pane="bottomLeft" activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3940,7 +3940,7 @@
         <v>198</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -3967,7 +3967,7 @@
         <v>285</v>
       </c>
       <c r="M63" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated the explanation file
Deleted ENF.CONT.COEN.ENFE.PR
</commit_message>
<xml_diff>
--- a/data/coding explanations_AI.xlsx
+++ b/data/coding explanations_AI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R working directory\ESG_availability\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA65468-88B3-427A-8DF9-90536EBDC5B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0463A6E-C1F0-44E8-A077-994058BE96DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B45AD726-65CD-4CBE-85A5-FE32CC3EFE12}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$135</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="327">
   <si>
     <t>cetsid</t>
   </si>
@@ -339,9 +339,6 @@
     <t>RL.EST</t>
   </si>
   <si>
-    <t>ENF.CONT.COEN.ENFE.PR</t>
-  </si>
-  <si>
     <t>VA.EST</t>
   </si>
   <si>
@@ -745,9 +742,6 @@
   </si>
   <si>
     <t>Rule of Law: Estimate</t>
-  </si>
-  <si>
-    <t>Enforcing contracts: Enforcement fees (% of claim)</t>
   </si>
   <si>
     <t>Voice and Accountability: Estimate</t>
@@ -1372,12 +1366,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C5F7576-3365-4997-A4EE-300F068BDE5E}">
-  <dimension ref="A1:M136"/>
+  <dimension ref="A1:M135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="M63" sqref="M63"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1392,40 +1386,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" t="s">
         <v>272</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>273</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>274</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>275</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>276</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>277</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>278</v>
       </c>
-      <c r="K1" t="s">
-        <v>279</v>
-      </c>
-      <c r="L1" t="s">
-        <v>280</v>
-      </c>
       <c r="M1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1436,7 +1430,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1463,10 +1457,10 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1477,7 +1471,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1504,10 +1498,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1518,7 +1512,7 @@
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1545,10 +1539,10 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1559,7 +1553,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1586,10 +1580,10 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1600,7 +1594,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1627,10 +1621,10 @@
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1641,7 +1635,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1668,10 +1662,10 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1682,7 +1676,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1709,10 +1703,10 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1723,7 +1717,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1750,10 +1744,10 @@
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1764,7 +1758,7 @@
         <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1791,10 +1785,10 @@
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1805,7 +1799,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1832,10 +1826,10 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1846,7 +1840,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1873,10 +1867,10 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1887,7 +1881,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1914,10 +1908,10 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1928,7 +1922,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1955,10 +1949,10 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1969,7 +1963,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1996,10 +1990,10 @@
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M15" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -2010,7 +2004,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2037,10 +2031,10 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M16" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -2051,7 +2045,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2078,10 +2072,10 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M17" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -2092,7 +2086,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2119,10 +2113,10 @@
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M18" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -2133,7 +2127,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2160,10 +2154,10 @@
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2174,7 +2168,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2201,10 +2195,10 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -2215,7 +2209,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2242,10 +2236,10 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -2256,7 +2250,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2283,10 +2277,10 @@
         <v>0</v>
       </c>
       <c r="L22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M22" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2297,7 +2291,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2324,10 +2318,10 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M23" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -2338,7 +2332,7 @@
         <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -2365,10 +2359,10 @@
         <v>0</v>
       </c>
       <c r="L24" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -2379,7 +2373,7 @@
         <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -2406,10 +2400,10 @@
         <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M25" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -2420,7 +2414,7 @@
         <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2447,10 +2441,10 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M26" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -2461,7 +2455,7 @@
         <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2488,10 +2482,10 @@
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M27" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -2502,7 +2496,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2529,10 +2523,10 @@
         <v>0</v>
       </c>
       <c r="L28" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M28" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -2543,7 +2537,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2570,10 +2564,10 @@
         <v>0</v>
       </c>
       <c r="L29" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M29" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -2584,7 +2578,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2611,10 +2605,10 @@
         <v>0</v>
       </c>
       <c r="L30" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M30" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -2625,7 +2619,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2652,10 +2646,10 @@
         <v>0</v>
       </c>
       <c r="L31" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M31" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -2666,7 +2660,7 @@
         <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2693,10 +2687,10 @@
         <v>0</v>
       </c>
       <c r="L32" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M32" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -2707,7 +2701,7 @@
         <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2734,10 +2728,10 @@
         <v>0</v>
       </c>
       <c r="L33" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M33" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -2748,7 +2742,7 @@
         <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -2775,10 +2769,10 @@
         <v>0</v>
       </c>
       <c r="L34" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M34" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -2789,7 +2783,7 @@
         <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -2816,10 +2810,10 @@
         <v>0</v>
       </c>
       <c r="L35" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M35" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -2830,7 +2824,7 @@
         <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -2857,10 +2851,10 @@
         <v>0</v>
       </c>
       <c r="L36" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M36" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -2871,7 +2865,7 @@
         <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -2898,10 +2892,10 @@
         <v>0</v>
       </c>
       <c r="L37" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M37" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -2912,7 +2906,7 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2939,10 +2933,10 @@
         <v>0</v>
       </c>
       <c r="L38" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M38" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -2953,7 +2947,7 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2980,10 +2974,10 @@
         <v>0</v>
       </c>
       <c r="L39" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M39" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
@@ -2994,7 +2988,7 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -3021,10 +3015,10 @@
         <v>0</v>
       </c>
       <c r="L40" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M40" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
@@ -3035,7 +3029,7 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -3062,10 +3056,10 @@
         <v>0</v>
       </c>
       <c r="L41" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M41" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -3076,7 +3070,7 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -3103,10 +3097,10 @@
         <v>0</v>
       </c>
       <c r="L42" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M42" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
@@ -3117,7 +3111,7 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -3144,10 +3138,10 @@
         <v>0</v>
       </c>
       <c r="L43" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M43" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
@@ -3158,7 +3152,7 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -3185,10 +3179,10 @@
         <v>0</v>
       </c>
       <c r="L44" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M44" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
@@ -3199,7 +3193,7 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -3226,10 +3220,10 @@
         <v>0</v>
       </c>
       <c r="L45" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M45" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
@@ -3240,7 +3234,7 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -3267,10 +3261,10 @@
         <v>0</v>
       </c>
       <c r="L46" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M46" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
@@ -3281,7 +3275,7 @@
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -3308,10 +3302,10 @@
         <v>0</v>
       </c>
       <c r="L47" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M47" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
@@ -3322,7 +3316,7 @@
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -3349,10 +3343,10 @@
         <v>0</v>
       </c>
       <c r="L48" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M48" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
@@ -3363,7 +3357,7 @@
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -3390,10 +3384,10 @@
         <v>0</v>
       </c>
       <c r="L49" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M49" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
@@ -3404,7 +3398,7 @@
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -3431,10 +3425,10 @@
         <v>0</v>
       </c>
       <c r="L50" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M50" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
@@ -3445,7 +3439,7 @@
         <v>57</v>
       </c>
       <c r="C51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3472,10 +3466,10 @@
         <v>0</v>
       </c>
       <c r="L51" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M51" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
@@ -3486,7 +3480,7 @@
         <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3513,10 +3507,10 @@
         <v>0</v>
       </c>
       <c r="L52" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M52" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
@@ -3527,7 +3521,7 @@
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -3554,10 +3548,10 @@
         <v>0</v>
       </c>
       <c r="L53" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M53" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
@@ -3568,7 +3562,7 @@
         <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -3595,10 +3589,10 @@
         <v>0</v>
       </c>
       <c r="L54" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M54" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
@@ -3609,7 +3603,7 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -3636,10 +3630,10 @@
         <v>0</v>
       </c>
       <c r="L55" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M55" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
@@ -3650,7 +3644,7 @@
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -3677,10 +3671,10 @@
         <v>0</v>
       </c>
       <c r="L56" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M56" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
@@ -3691,7 +3685,7 @@
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -3718,10 +3712,10 @@
         <v>0</v>
       </c>
       <c r="L57" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M57" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
@@ -3732,7 +3726,7 @@
         <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -3759,10 +3753,10 @@
         <v>0</v>
       </c>
       <c r="L58" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M58" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
@@ -3773,7 +3767,7 @@
         <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -3800,10 +3794,10 @@
         <v>0</v>
       </c>
       <c r="L59" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M59" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
@@ -3814,7 +3808,7 @@
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -3841,10 +3835,10 @@
         <v>0</v>
       </c>
       <c r="L60" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M60" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
@@ -3855,7 +3849,7 @@
         <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -3882,10 +3876,10 @@
         <v>0</v>
       </c>
       <c r="L61" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M61" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
@@ -3896,7 +3890,7 @@
         <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -3923,10 +3917,10 @@
         <v>0</v>
       </c>
       <c r="L62" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M62" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
@@ -3937,7 +3931,7 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -3964,10 +3958,10 @@
         <v>0</v>
       </c>
       <c r="L63" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M63" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
@@ -3978,7 +3972,7 @@
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -4005,10 +3999,10 @@
         <v>0</v>
       </c>
       <c r="L64" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M64" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
@@ -4019,7 +4013,7 @@
         <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -4046,10 +4040,10 @@
         <v>0</v>
       </c>
       <c r="L65" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M65" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
@@ -4060,7 +4054,7 @@
         <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -4087,10 +4081,10 @@
         <v>0</v>
       </c>
       <c r="L66" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M66" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
@@ -4101,7 +4095,7 @@
         <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -4128,10 +4122,10 @@
         <v>0</v>
       </c>
       <c r="L67" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M67" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
@@ -4142,7 +4136,7 @@
         <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -4169,10 +4163,10 @@
         <v>0</v>
       </c>
       <c r="L68" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M68" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
@@ -4183,7 +4177,7 @@
         <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -4210,10 +4204,10 @@
         <v>0</v>
       </c>
       <c r="L69" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M69" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
@@ -4224,7 +4218,7 @@
         <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -4251,10 +4245,10 @@
         <v>0</v>
       </c>
       <c r="L70" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M70" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
@@ -4265,7 +4259,7 @@
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -4292,10 +4286,10 @@
         <v>0</v>
       </c>
       <c r="L71" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M71" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
@@ -4306,7 +4300,7 @@
         <v>2</v>
       </c>
       <c r="C72" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -4333,7 +4327,7 @@
         <v>0</v>
       </c>
       <c r="L72" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
@@ -4344,7 +4338,7 @@
         <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -4371,10 +4365,10 @@
         <v>0</v>
       </c>
       <c r="L73" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M73" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
@@ -4385,7 +4379,7 @@
         <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -4412,10 +4406,10 @@
         <v>0</v>
       </c>
       <c r="L74" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M74" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
@@ -4426,7 +4420,7 @@
         <v>11</v>
       </c>
       <c r="C75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -4453,10 +4447,10 @@
         <v>0</v>
       </c>
       <c r="L75" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M75" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
@@ -4467,7 +4461,7 @@
         <v>2</v>
       </c>
       <c r="C76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -4494,10 +4488,10 @@
         <v>0</v>
       </c>
       <c r="L76" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M76" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
@@ -4508,7 +4502,7 @@
         <v>14</v>
       </c>
       <c r="C77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -4535,10 +4529,10 @@
         <v>0</v>
       </c>
       <c r="L77" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M77" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
@@ -4549,7 +4543,7 @@
         <v>14</v>
       </c>
       <c r="C78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -4576,10 +4570,10 @@
         <v>0</v>
       </c>
       <c r="L78" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M78" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
@@ -4590,7 +4584,7 @@
         <v>2</v>
       </c>
       <c r="C79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -4617,10 +4611,10 @@
         <v>0</v>
       </c>
       <c r="L79" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M79" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
@@ -4631,7 +4625,7 @@
         <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -4658,10 +4652,10 @@
         <v>0</v>
       </c>
       <c r="L80" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M80" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
@@ -4672,7 +4666,7 @@
         <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -4699,10 +4693,10 @@
         <v>0</v>
       </c>
       <c r="L81" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M81" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
@@ -4713,7 +4707,7 @@
         <v>2</v>
       </c>
       <c r="C82" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -4740,10 +4734,10 @@
         <v>0</v>
       </c>
       <c r="L82" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M82" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
@@ -4754,7 +4748,7 @@
         <v>2</v>
       </c>
       <c r="C83" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -4781,10 +4775,10 @@
         <v>0</v>
       </c>
       <c r="L83" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M83" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
@@ -4795,7 +4789,7 @@
         <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -4822,10 +4816,10 @@
         <v>0</v>
       </c>
       <c r="L84" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M84" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
@@ -4836,7 +4830,7 @@
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -4863,10 +4857,10 @@
         <v>0</v>
       </c>
       <c r="L85" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M85" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.3">
@@ -4877,7 +4871,7 @@
         <v>3</v>
       </c>
       <c r="C86" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -4904,10 +4898,10 @@
         <v>0</v>
       </c>
       <c r="L86" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M86" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
@@ -4918,7 +4912,7 @@
         <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -4945,10 +4939,10 @@
         <v>0</v>
       </c>
       <c r="L87" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M87" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.3">
@@ -4959,7 +4953,7 @@
         <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -4986,10 +4980,10 @@
         <v>0</v>
       </c>
       <c r="L88" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M88" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.3">
@@ -5000,7 +4994,7 @@
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -5027,10 +5021,10 @@
         <v>0</v>
       </c>
       <c r="L89" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M89" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.3">
@@ -5041,7 +5035,7 @@
         <v>32</v>
       </c>
       <c r="C90" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -5068,10 +5062,10 @@
         <v>0</v>
       </c>
       <c r="L90" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M90" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.3">
@@ -5082,7 +5076,7 @@
         <v>2</v>
       </c>
       <c r="C91" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -5109,10 +5103,10 @@
         <v>0</v>
       </c>
       <c r="L91" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M91" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.3">
@@ -5123,7 +5117,7 @@
         <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -5150,10 +5144,10 @@
         <v>0</v>
       </c>
       <c r="L92" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M92" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.3">
@@ -5164,7 +5158,7 @@
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -5191,10 +5185,10 @@
         <v>0</v>
       </c>
       <c r="L93" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M93" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.3">
@@ -5205,7 +5199,7 @@
         <v>11</v>
       </c>
       <c r="C94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -5232,10 +5226,10 @@
         <v>0</v>
       </c>
       <c r="L94" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M94" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.3">
@@ -5246,7 +5240,7 @@
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -5273,10 +5267,10 @@
         <v>0</v>
       </c>
       <c r="L95" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M95" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.3">
@@ -5287,7 +5281,7 @@
         <v>11</v>
       </c>
       <c r="C96" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -5314,10 +5308,10 @@
         <v>0</v>
       </c>
       <c r="L96" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M96" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.3">
@@ -5328,7 +5322,7 @@
         <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -5355,10 +5349,10 @@
         <v>0</v>
       </c>
       <c r="L97" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M97" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.3">
@@ -5369,7 +5363,7 @@
         <v>11</v>
       </c>
       <c r="C98" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -5396,10 +5390,10 @@
         <v>0</v>
       </c>
       <c r="L98" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M98" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.3">
@@ -5410,7 +5404,7 @@
         <v>2</v>
       </c>
       <c r="C99" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -5437,10 +5431,10 @@
         <v>0</v>
       </c>
       <c r="L99" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M99" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.3">
@@ -5451,7 +5445,7 @@
         <v>3</v>
       </c>
       <c r="C100" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -5478,10 +5472,10 @@
         <v>0</v>
       </c>
       <c r="L100" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M100" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.3">
@@ -5492,7 +5486,7 @@
         <v>3</v>
       </c>
       <c r="C101" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -5519,10 +5513,10 @@
         <v>0</v>
       </c>
       <c r="L101" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M101" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.3">
@@ -5530,10 +5524,10 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C102" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -5560,10 +5554,10 @@
         <v>0</v>
       </c>
       <c r="L102" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M102" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.3">
@@ -5571,10 +5565,10 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C103" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -5583,7 +5577,7 @@
         <v>0</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -5604,7 +5598,7 @@
         <v>283</v>
       </c>
       <c r="M103" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.3">
@@ -5612,10 +5606,10 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -5624,7 +5618,7 @@
         <v>0</v>
       </c>
       <c r="F104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -5642,10 +5636,10 @@
         <v>0</v>
       </c>
       <c r="L104" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="M104" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.3">
@@ -5653,10 +5647,10 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C105" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -5677,16 +5671,16 @@
         <v>0</v>
       </c>
       <c r="J105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K105">
         <v>0</v>
       </c>
       <c r="L105" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="M105" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.3">
@@ -5697,7 +5691,7 @@
         <v>2</v>
       </c>
       <c r="C106" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -5706,7 +5700,7 @@
         <v>0</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -5718,16 +5712,16 @@
         <v>0</v>
       </c>
       <c r="J106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K106">
         <v>0</v>
       </c>
       <c r="L106" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M106" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.3">
@@ -5738,7 +5732,7 @@
         <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -5765,10 +5759,10 @@
         <v>0</v>
       </c>
       <c r="L107" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M107" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.3">
@@ -5779,7 +5773,7 @@
         <v>2</v>
       </c>
       <c r="C108" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -5788,7 +5782,7 @@
         <v>0</v>
       </c>
       <c r="F108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -5806,10 +5800,10 @@
         <v>0</v>
       </c>
       <c r="L108" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="M108" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
@@ -5820,7 +5814,7 @@
         <v>2</v>
       </c>
       <c r="C109" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -5838,19 +5832,19 @@
         <v>0</v>
       </c>
       <c r="I109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K109">
         <v>0</v>
       </c>
       <c r="L109" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M109" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.3">
@@ -5861,7 +5855,7 @@
         <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -5879,19 +5873,19 @@
         <v>0</v>
       </c>
       <c r="I110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K110">
         <v>0</v>
       </c>
       <c r="L110" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="M110" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.3">
@@ -5902,7 +5896,7 @@
         <v>2</v>
       </c>
       <c r="C111" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -5920,19 +5914,19 @@
         <v>0</v>
       </c>
       <c r="I111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K111">
         <v>0</v>
       </c>
       <c r="L111" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="M111" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
@@ -5943,7 +5937,7 @@
         <v>2</v>
       </c>
       <c r="C112" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -5970,10 +5964,10 @@
         <v>0</v>
       </c>
       <c r="L112" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M112" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.3">
@@ -5984,7 +5978,7 @@
         <v>2</v>
       </c>
       <c r="C113" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -5993,7 +5987,7 @@
         <v>0</v>
       </c>
       <c r="F113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -6002,19 +5996,19 @@
         <v>0</v>
       </c>
       <c r="I113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K113">
         <v>0</v>
       </c>
       <c r="L113" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="M113" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.3">
@@ -6025,7 +6019,7 @@
         <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -6052,10 +6046,10 @@
         <v>0</v>
       </c>
       <c r="L114" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="M114" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.3">
@@ -6066,7 +6060,7 @@
         <v>2</v>
       </c>
       <c r="C115" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -6075,7 +6069,7 @@
         <v>0</v>
       </c>
       <c r="F115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -6093,10 +6087,10 @@
         <v>0</v>
       </c>
       <c r="L115" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="M115" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.3">
@@ -6107,7 +6101,7 @@
         <v>2</v>
       </c>
       <c r="C116" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -6125,19 +6119,19 @@
         <v>0</v>
       </c>
       <c r="I116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K116">
         <v>0</v>
       </c>
       <c r="L116" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="M116" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.3">
@@ -6148,7 +6142,7 @@
         <v>2</v>
       </c>
       <c r="C117" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D117">
         <v>0</v>
@@ -6166,19 +6160,19 @@
         <v>0</v>
       </c>
       <c r="I117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K117">
         <v>0</v>
       </c>
       <c r="L117" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="M117" t="s">
-        <v>321</v>
+        <v>296</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.3">
@@ -6189,7 +6183,7 @@
         <v>2</v>
       </c>
       <c r="C118" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -6210,7 +6204,7 @@
         <v>0</v>
       </c>
       <c r="J118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K118">
         <v>0</v>
@@ -6219,7 +6213,7 @@
         <v>282</v>
       </c>
       <c r="M118" t="s">
-        <v>298</v>
+        <v>321</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.3">
@@ -6230,7 +6224,7 @@
         <v>2</v>
       </c>
       <c r="C119" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -6251,16 +6245,16 @@
         <v>0</v>
       </c>
       <c r="J119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K119">
         <v>0</v>
       </c>
       <c r="L119" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="M119" t="s">
-        <v>323</v>
+        <v>296</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.3">
@@ -6271,7 +6265,7 @@
         <v>2</v>
       </c>
       <c r="C120" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -6298,10 +6292,10 @@
         <v>0</v>
       </c>
       <c r="L120" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="M120" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.3">
@@ -6309,13 +6303,13 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C121" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E121">
         <v>0</v>
@@ -6339,10 +6333,10 @@
         <v>0</v>
       </c>
       <c r="L121" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M121" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.3">
@@ -6350,13 +6344,13 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C122" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -6380,10 +6374,10 @@
         <v>0</v>
       </c>
       <c r="L122" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="M122" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.3">
@@ -6394,7 +6388,7 @@
         <v>2</v>
       </c>
       <c r="C123" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -6421,10 +6415,10 @@
         <v>0</v>
       </c>
       <c r="L123" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M123" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.3">
@@ -6432,13 +6426,13 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C124" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124">
         <v>0</v>
@@ -6462,10 +6456,10 @@
         <v>0</v>
       </c>
       <c r="L124" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M124" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.3">
@@ -6476,7 +6470,7 @@
         <v>11</v>
       </c>
       <c r="C125" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D125">
         <v>1</v>
@@ -6503,10 +6497,10 @@
         <v>0</v>
       </c>
       <c r="L125" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M125" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.3">
@@ -6514,13 +6508,13 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C126" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D126">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E126">
         <v>0</v>
@@ -6535,19 +6529,19 @@
         <v>0</v>
       </c>
       <c r="I126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K126">
         <v>0</v>
       </c>
       <c r="L126" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="M126" t="s">
-        <v>297</v>
+        <v>319</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.3">
@@ -6558,7 +6552,7 @@
         <v>2</v>
       </c>
       <c r="C127" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -6576,7 +6570,7 @@
         <v>0</v>
       </c>
       <c r="I127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J127">
         <v>1</v>
@@ -6585,10 +6579,10 @@
         <v>0</v>
       </c>
       <c r="L127" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="M127" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.3">
@@ -6599,7 +6593,7 @@
         <v>2</v>
       </c>
       <c r="C128" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D128">
         <v>0</v>
@@ -6620,16 +6614,16 @@
         <v>0</v>
       </c>
       <c r="J128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K128">
         <v>0</v>
       </c>
       <c r="L128" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M128" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.3">
@@ -6640,7 +6634,7 @@
         <v>2</v>
       </c>
       <c r="C129" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -6649,7 +6643,7 @@
         <v>0</v>
       </c>
       <c r="F129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G129">
         <v>0</v>
@@ -6667,10 +6661,10 @@
         <v>0</v>
       </c>
       <c r="L129" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="M129" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.3">
@@ -6681,7 +6675,7 @@
         <v>2</v>
       </c>
       <c r="C130" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D130">
         <v>0</v>
@@ -6690,7 +6684,7 @@
         <v>0</v>
       </c>
       <c r="F130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G130">
         <v>0</v>
@@ -6708,10 +6702,10 @@
         <v>0</v>
       </c>
       <c r="L130" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="M130" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.3">
@@ -6722,7 +6716,7 @@
         <v>2</v>
       </c>
       <c r="C131" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D131">
         <v>0</v>
@@ -6743,16 +6737,16 @@
         <v>0</v>
       </c>
       <c r="J131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K131">
         <v>0</v>
       </c>
       <c r="L131" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="M131" t="s">
-        <v>298</v>
+        <v>320</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.3">
@@ -6763,7 +6757,7 @@
         <v>2</v>
       </c>
       <c r="C132" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D132">
         <v>0</v>
@@ -6790,10 +6784,10 @@
         <v>0</v>
       </c>
       <c r="L132" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M132" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.3">
@@ -6804,7 +6798,7 @@
         <v>2</v>
       </c>
       <c r="C133" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D133">
         <v>0</v>
@@ -6813,7 +6807,7 @@
         <v>0</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G133">
         <v>0</v>
@@ -6825,16 +6819,16 @@
         <v>0</v>
       </c>
       <c r="J133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K133">
         <v>0</v>
       </c>
       <c r="L133" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="M133" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.3">
@@ -6845,7 +6839,7 @@
         <v>2</v>
       </c>
       <c r="C134" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D134">
         <v>0</v>
@@ -6872,10 +6866,10 @@
         <v>0</v>
       </c>
       <c r="L134" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="M134" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.3">
@@ -6886,7 +6880,7 @@
         <v>2</v>
       </c>
       <c r="C135" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D135">
         <v>0</v>
@@ -6895,7 +6889,7 @@
         <v>0</v>
       </c>
       <c r="F135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G135">
         <v>0</v>
@@ -6904,60 +6898,19 @@
         <v>0</v>
       </c>
       <c r="I135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K135">
         <v>0</v>
       </c>
       <c r="L135" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="M135" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>135</v>
-      </c>
-      <c r="B136">
-        <v>2</v>
-      </c>
-      <c r="C136" t="s">
-        <v>271</v>
-      </c>
-      <c r="D136">
-        <v>0</v>
-      </c>
-      <c r="E136">
-        <v>0</v>
-      </c>
-      <c r="F136">
-        <v>0</v>
-      </c>
-      <c r="G136">
-        <v>0</v>
-      </c>
-      <c r="H136">
-        <v>0</v>
-      </c>
-      <c r="I136">
-        <v>1</v>
-      </c>
-      <c r="J136">
-        <v>1</v>
-      </c>
-      <c r="K136">
-        <v>0</v>
-      </c>
-      <c r="L136" t="s">
-        <v>288</v>
-      </c>
-      <c r="M136" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>